<commit_message>
Update analysis document with re-run data
</commit_message>
<xml_diff>
--- a/ICS411/Assignment3/report/analysis.xlsx
+++ b/ICS411/Assignment3/report/analysis.xlsx
@@ -645,9 +645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -685,16 +683,16 @@
         <v>5</v>
       </c>
       <c r="C3" s="6">
-        <v>404720</v>
+        <v>2268578</v>
       </c>
       <c r="D3" s="4">
-        <v>25814</v>
+        <v>2261252</v>
       </c>
       <c r="E3" s="6">
-        <v>2268650</v>
+        <v>2268644</v>
       </c>
       <c r="F3" s="4">
-        <v>2261324</v>
+        <v>2261318</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -702,16 +700,16 @@
         <v>6</v>
       </c>
       <c r="C4" s="6">
-        <v>1095817</v>
+        <v>4823533</v>
       </c>
       <c r="D4" s="4">
-        <v>338337</v>
+        <v>4809213</v>
       </c>
       <c r="E4" s="6">
-        <v>6544308</v>
+        <v>6400938</v>
       </c>
       <c r="F4" s="4">
-        <v>6532036</v>
+        <v>6388496</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -719,10 +717,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="6">
-        <v>20779</v>
+        <v>2178867</v>
       </c>
       <c r="D5" s="4">
-        <v>20779</v>
+        <v>2178867</v>
       </c>
       <c r="E5" s="6">
         <v>2178867</v>
@@ -736,16 +734,16 @@
         <v>8</v>
       </c>
       <c r="C6" s="6">
-        <v>10763</v>
+        <v>2616</v>
       </c>
       <c r="D6" s="4">
-        <v>3146</v>
+        <v>2469</v>
       </c>
       <c r="E6" s="6">
-        <v>3440</v>
+        <v>2472</v>
       </c>
       <c r="F6" s="4">
-        <v>2358</v>
+        <v>2315</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -753,16 +751,16 @@
         <v>9</v>
       </c>
       <c r="C7" s="6">
-        <v>4708</v>
+        <v>2771</v>
       </c>
       <c r="D7" s="4">
-        <v>3068</v>
+        <v>2507</v>
       </c>
       <c r="E7" s="6">
-        <v>68614</v>
+        <v>64953</v>
       </c>
       <c r="F7" s="4">
-        <v>70938</v>
+        <v>48472</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -790,7 +788,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="4">
-        <v>1309</v>
+        <v>20030</v>
       </c>
       <c r="E9" s="6">
         <v>0</v>
@@ -804,16 +802,16 @@
         <v>12</v>
       </c>
       <c r="C10" s="6">
-        <v>404720</v>
+        <v>2268578</v>
       </c>
       <c r="D10" s="4">
-        <v>25814</v>
+        <v>2261252</v>
       </c>
       <c r="E10" s="6">
-        <v>2268650</v>
+        <v>2268644</v>
       </c>
       <c r="F10" s="4">
-        <v>2261324</v>
+        <v>2261318</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -824,7 +822,7 @@
         <v>20103</v>
       </c>
       <c r="D11" s="4">
-        <v>1309</v>
+        <v>20030</v>
       </c>
       <c r="E11" s="6">
         <v>20103</v>
@@ -838,10 +836,10 @@
         <v>14</v>
       </c>
       <c r="C12" s="6">
-        <v>1309</v>
+        <v>20030</v>
       </c>
       <c r="D12" s="4">
-        <v>1309</v>
+        <v>20030</v>
       </c>
       <c r="E12" s="6">
         <v>20030</v>
@@ -858,7 +856,7 @@
         <v>40206</v>
       </c>
       <c r="D13" s="4">
-        <v>2618</v>
+        <v>40060</v>
       </c>
       <c r="E13" s="6">
         <v>40206</v>
@@ -878,10 +876,10 @@
         <v>1</v>
       </c>
       <c r="E14" s="6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -895,10 +893,10 @@
         <v>1</v>
       </c>
       <c r="E15" s="6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -906,16 +904,16 @@
         <v>17</v>
       </c>
       <c r="C16" s="7">
-        <v>362283008</v>
+        <v>555220992</v>
       </c>
       <c r="D16" s="4">
-        <v>548405248</v>
+        <v>555745280</v>
       </c>
       <c r="E16" s="7">
-        <v>2583691264</v>
+        <v>2337800192</v>
       </c>
       <c r="F16" s="4">
-        <v>2457862144</v>
+        <v>2285895680</v>
       </c>
     </row>
   </sheetData>

</xml_diff>